<commit_message>
all login changes commited with adding 2 more cases
</commit_message>
<xml_diff>
--- a/testdata/LoginIneurone.xlsx
+++ b/testdata/LoginIneurone.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="loginCred" sheetId="1" r:id="rId1"/>
+    <sheet name="inValidloginCred" sheetId="2" r:id="rId2"/>
+    <sheet name="loginCredMultiway" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Password</t>
   </si>
@@ -26,13 +28,64 @@
   </si>
   <si>
     <t>ineuron</t>
+  </si>
+  <si>
+    <t>ineu@ineuron.ai</t>
+  </si>
+  <si>
+    <t>shdfsdf</t>
+  </si>
+  <si>
+    <t>ineuw@gmail.com</t>
+  </si>
+  <si>
+    <t>sdfsdgs</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>UserEmail</t>
+  </si>
+  <si>
+    <t>UserPass</t>
+  </si>
+  <si>
+    <t>ValidCred</t>
+  </si>
+  <si>
+    <t>admin@email.com</t>
+  </si>
+  <si>
+    <t>admin@123</t>
+  </si>
+  <si>
+    <t>BothInvalid</t>
+  </si>
+  <si>
+    <t>admin21@123</t>
+  </si>
+  <si>
+    <t>admin12@email.com</t>
+  </si>
+  <si>
+    <t>ValidEmailInvalidPass</t>
+  </si>
+  <si>
+    <t>InvalidEmailValidPass</t>
+  </si>
+  <si>
+    <t>BlankEmailValidPass</t>
+  </si>
+  <si>
+    <t>ValidEmailBlankPass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,6 +97,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -85,10 +146,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -396,8 +458,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,24 +507,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="C4" r:id="rId6"/>
+    <hyperlink ref="B5" r:id="rId7"/>
+    <hyperlink ref="C5" r:id="rId8"/>
+    <hyperlink ref="C6" r:id="rId9"/>
+    <hyperlink ref="B7" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>